<commit_message>
UIX and features implementation & Dashboard
</commit_message>
<xml_diff>
--- a/Import Sales.xlsx
+++ b/Import Sales.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyProjects\Customers\Twiga Cement\twiga_sales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DevProjects\Python\django\twiga_sales\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="103">
   <si>
     <t>Transaction Date</t>
   </si>
@@ -170,24 +170,6 @@
     <t>DN100025</t>
   </si>
   <si>
-    <t>DN100026</t>
-  </si>
-  <si>
-    <t>DN100027</t>
-  </si>
-  <si>
-    <t>DN100028</t>
-  </si>
-  <si>
-    <t>DN100029</t>
-  </si>
-  <si>
-    <t>DN100030</t>
-  </si>
-  <si>
-    <t>DN100031</t>
-  </si>
-  <si>
     <t>T101AAA</t>
   </si>
   <si>
@@ -269,24 +251,6 @@
     <t>TI800025</t>
   </si>
   <si>
-    <t>TI800026</t>
-  </si>
-  <si>
-    <t>TI800027</t>
-  </si>
-  <si>
-    <t>TI800028</t>
-  </si>
-  <si>
-    <t>TI800029</t>
-  </si>
-  <si>
-    <t>TI800030</t>
-  </si>
-  <si>
-    <t>TI800031</t>
-  </si>
-  <si>
     <t>SON3000001</t>
   </si>
   <si>
@@ -360,24 +324,6 @@
   </si>
   <si>
     <t>SON3000025</t>
-  </si>
-  <si>
-    <t>SON3000026</t>
-  </si>
-  <si>
-    <t>SON3000027</t>
-  </si>
-  <si>
-    <t>SON3000028</t>
-  </si>
-  <si>
-    <t>SON3000029</t>
-  </si>
-  <si>
-    <t>SON3000030</t>
-  </si>
-  <si>
-    <t>SON3000031</t>
   </si>
   <si>
     <t>Uganda</t>
@@ -392,7 +338,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -727,10 +673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -790,13 +736,13 @@
         <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F2" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="G2" t="s">
         <v>10</v>
@@ -808,7 +754,7 @@
         <v>50000</v>
       </c>
       <c r="J2" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -822,13 +768,13 @@
         <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="F3" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="G3" t="s">
         <v>10</v>
@@ -840,7 +786,7 @@
         <v>70002</v>
       </c>
       <c r="J3" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -854,13 +800,13 @@
         <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E4" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F4" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="G4" t="s">
         <v>10</v>
@@ -872,7 +818,7 @@
         <v>50000</v>
       </c>
       <c r="J4" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -886,13 +832,13 @@
         <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="F5" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="G5" t="s">
         <v>10</v>
@@ -918,13 +864,13 @@
         <v>27</v>
       </c>
       <c r="D6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" t="s">
         <v>54</v>
       </c>
-      <c r="E6" t="s">
-        <v>60</v>
-      </c>
       <c r="F6" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="G6" t="s">
         <v>10</v>
@@ -950,13 +896,13 @@
         <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E7" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F7" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="G7" t="s">
         <v>10</v>
@@ -968,7 +914,7 @@
         <v>50000</v>
       </c>
       <c r="J7" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -982,13 +928,13 @@
         <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E8" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="F8" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="G8" t="s">
         <v>10</v>
@@ -1000,7 +946,7 @@
         <v>52425</v>
       </c>
       <c r="J8" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1014,13 +960,13 @@
         <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E9" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F9" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="G9" t="s">
         <v>10</v>
@@ -1032,7 +978,7 @@
         <v>52425</v>
       </c>
       <c r="J9" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1046,13 +992,13 @@
         <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E10" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F10" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="G10" t="s">
         <v>10</v>
@@ -1064,7 +1010,7 @@
         <v>70002</v>
       </c>
       <c r="J10" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1078,13 +1024,13 @@
         <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E11" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F11" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="G11" t="s">
         <v>10</v>
@@ -1110,13 +1056,13 @@
         <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E12" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F12" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="G12" t="s">
         <v>10</v>
@@ -1128,7 +1074,7 @@
         <v>50000</v>
       </c>
       <c r="J12" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1142,13 +1088,13 @@
         <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E13" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="F13" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="G13" t="s">
         <v>10</v>
@@ -1160,7 +1106,7 @@
         <v>70002</v>
       </c>
       <c r="J13" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1174,13 +1120,13 @@
         <v>35</v>
       </c>
       <c r="D14" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E14" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F14" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="G14" t="s">
         <v>10</v>
@@ -1192,7 +1138,7 @@
         <v>50000</v>
       </c>
       <c r="J14" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1206,13 +1152,13 @@
         <v>36</v>
       </c>
       <c r="D15" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E15" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F15" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="G15" t="s">
         <v>10</v>
@@ -1238,13 +1184,13 @@
         <v>37</v>
       </c>
       <c r="D16" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E16" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F16" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="G16" t="s">
         <v>10</v>
@@ -1270,13 +1216,13 @@
         <v>38</v>
       </c>
       <c r="D17" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E17" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F17" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="G17" t="s">
         <v>10</v>
@@ -1288,7 +1234,7 @@
         <v>50000</v>
       </c>
       <c r="J17" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1302,13 +1248,13 @@
         <v>39</v>
       </c>
       <c r="D18" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E18" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F18" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="G18" t="s">
         <v>10</v>
@@ -1320,7 +1266,7 @@
         <v>70002</v>
       </c>
       <c r="J18" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1334,13 +1280,13 @@
         <v>40</v>
       </c>
       <c r="D19" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E19" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F19" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="G19" t="s">
         <v>10</v>
@@ -1352,7 +1298,7 @@
         <v>50000</v>
       </c>
       <c r="J19" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1366,13 +1312,13 @@
         <v>41</v>
       </c>
       <c r="D20" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E20" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F20" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="G20" t="s">
         <v>10</v>
@@ -1384,7 +1330,7 @@
         <v>52425</v>
       </c>
       <c r="J20" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1398,13 +1344,13 @@
         <v>42</v>
       </c>
       <c r="D21" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E21" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F21" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="G21" t="s">
         <v>10</v>
@@ -1430,13 +1376,13 @@
         <v>43</v>
       </c>
       <c r="D22" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E22" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F22" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="G22" t="s">
         <v>10</v>
@@ -1462,13 +1408,13 @@
         <v>44</v>
       </c>
       <c r="D23" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E23" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F23" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="G23" t="s">
         <v>10</v>
@@ -1480,7 +1426,7 @@
         <v>70002</v>
       </c>
       <c r="J23" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1494,13 +1440,13 @@
         <v>45</v>
       </c>
       <c r="D24" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E24" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F24" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="G24" t="s">
         <v>10</v>
@@ -1526,13 +1472,13 @@
         <v>46</v>
       </c>
       <c r="D25" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E25" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F25" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="G25" t="s">
         <v>10</v>
@@ -1558,13 +1504,13 @@
         <v>47</v>
       </c>
       <c r="D26" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E26" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="F26" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="G26" t="s">
         <v>10</v>
@@ -1576,199 +1522,7 @@
         <v>52425</v>
       </c>
       <c r="J26" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
-        <v>43911</v>
-      </c>
-      <c r="B27" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" t="s">
-        <v>48</v>
-      </c>
-      <c r="D27" t="s">
-        <v>54</v>
-      </c>
-      <c r="E27" t="s">
-        <v>81</v>
-      </c>
-      <c r="F27" t="s">
-        <v>112</v>
-      </c>
-      <c r="G27" t="s">
-        <v>10</v>
-      </c>
-      <c r="H27">
-        <v>40</v>
-      </c>
-      <c r="I27">
-        <v>70002</v>
-      </c>
-      <c r="J27" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
-        <v>43912</v>
-      </c>
-      <c r="B28" t="s">
-        <v>14</v>
-      </c>
-      <c r="C28" t="s">
-        <v>49</v>
-      </c>
-      <c r="D28" t="s">
-        <v>55</v>
-      </c>
-      <c r="E28" t="s">
-        <v>82</v>
-      </c>
-      <c r="F28" t="s">
-        <v>113</v>
-      </c>
-      <c r="G28" t="s">
-        <v>10</v>
-      </c>
-      <c r="H28">
-        <v>87</v>
-      </c>
-      <c r="I28">
-        <v>50000</v>
-      </c>
-      <c r="J28" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
-        <v>43913</v>
-      </c>
-      <c r="B29" t="s">
-        <v>15</v>
-      </c>
-      <c r="C29" t="s">
-        <v>50</v>
-      </c>
-      <c r="D29" t="s">
-        <v>54</v>
-      </c>
-      <c r="E29" t="s">
-        <v>83</v>
-      </c>
-      <c r="F29" t="s">
-        <v>114</v>
-      </c>
-      <c r="G29" t="s">
-        <v>10</v>
-      </c>
-      <c r="H29">
-        <v>89</v>
-      </c>
-      <c r="I29">
-        <v>50000</v>
-      </c>
-      <c r="J29" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
-        <v>43914</v>
-      </c>
-      <c r="B30" t="s">
-        <v>16</v>
-      </c>
-      <c r="C30" t="s">
-        <v>51</v>
-      </c>
-      <c r="D30" t="s">
-        <v>54</v>
-      </c>
-      <c r="E30" t="s">
-        <v>84</v>
-      </c>
-      <c r="F30" t="s">
-        <v>115</v>
-      </c>
-      <c r="G30" t="s">
-        <v>10</v>
-      </c>
-      <c r="H30">
-        <v>40</v>
-      </c>
-      <c r="I30">
-        <v>70002</v>
-      </c>
-      <c r="J30" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
-        <v>43915</v>
-      </c>
-      <c r="B31" t="s">
-        <v>15</v>
-      </c>
-      <c r="C31" t="s">
-        <v>52</v>
-      </c>
-      <c r="D31" t="s">
-        <v>55</v>
-      </c>
-      <c r="E31" t="s">
-        <v>85</v>
-      </c>
-      <c r="F31" t="s">
-        <v>116</v>
-      </c>
-      <c r="G31" t="s">
-        <v>10</v>
-      </c>
-      <c r="H31">
-        <v>87</v>
-      </c>
-      <c r="I31">
-        <v>50000</v>
-      </c>
-      <c r="J31" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
-        <v>43916</v>
-      </c>
-      <c r="B32" t="s">
-        <v>12</v>
-      </c>
-      <c r="C32" t="s">
-        <v>53</v>
-      </c>
-      <c r="D32" t="s">
-        <v>54</v>
-      </c>
-      <c r="E32" t="s">
-        <v>86</v>
-      </c>
-      <c r="F32" t="s">
-        <v>117</v>
-      </c>
-      <c r="G32" t="s">
-        <v>10</v>
-      </c>
-      <c r="H32">
-        <v>100</v>
-      </c>
-      <c r="I32">
-        <v>52425</v>
-      </c>
-      <c r="J32" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>